<commit_message>
docs: add some content
</commit_message>
<xml_diff>
--- a/12月前端任务评估.xlsx
+++ b/12月前端任务评估.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12465"/>
+    <workbookView windowWidth="20760" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="待定要做的工时" sheetId="11" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83">
   <si>
     <t>优先级</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF262626"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>【3535-老客户拉新】
 二级分销老带新</t>
     </r>
@@ -327,6 +333,21 @@
   <si>
     <t>大B希望能够创建更多的组合促销活动（现在是30条），便于更多的商品进行组合去做活动销售。</t>
   </si>
+  <si>
+    <t>套餐促销</t>
+  </si>
+  <si>
+    <t>1 应用中心设置。
+2 上了列表，筛选、显示。
+3 新增/修改商品，成分模块，单位、起订量、限定量。
+4 商品详情展示。
+5 代下单、订单修改、订单详情时展示调整，可能要注意验证一下促销逻辑是否正常。
+6 出库逻辑调整，要注意电子面单逻辑是否正常。
+7 库存无法选择商品，要置灰，逻辑上可能要处理，不只一处，采购、盘点、退货都要处理。</t>
+  </si>
+  <si>
+    <t>1 没有说明，订单修改是否有影响。</t>
+  </si>
 </sst>
 </file>
 
@@ -334,8 +355,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -375,9 +396,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -391,7 +411,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -406,98 +426,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -519,6 +448,98 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF262626"/>
       <name val="Times New Roman"/>
@@ -534,187 +555,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -876,45 +897,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -936,6 +918,39 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -964,11 +979,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -978,10 +999,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -990,137 +1011,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1146,9 +1167,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1188,15 +1206,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1208,9 +1217,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1602,14 +1608,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:XFD45"/>
+  <dimension ref="A1:XFD66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J36" sqref="J36:J37"/>
+      <selection pane="bottomRight" activeCell="E57" sqref="E57:E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
@@ -1641,20 +1647,20 @@
         <v>3</v>
       </c>
       <c r="E1" s="8"/>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="6" t="s">
         <v>8</v>
       </c>
@@ -1662,16 +1668,16 @@
     <row r="2" s="1" customFormat="1" ht="18" spans="1:12">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="32" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="6" t="s">
@@ -1680,641 +1686,641 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="72" customHeight="1" spans="1:12">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="22">
+      <c r="F3" s="20"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="21">
         <f>SUM(G3:G7)</f>
         <v>64</v>
       </c>
-      <c r="I3" s="34">
+      <c r="I3" s="29">
         <v>64</v>
       </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="37"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="32"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="63" customHeight="1" spans="1:12">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="19" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="37"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="32"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="19" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="18">
         <v>48</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="37"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="32"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A6" s="23"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="19" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="37"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="32"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="75" customHeight="1" spans="1:12">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="19" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="18">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="37"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="32"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="72" customHeight="1" spans="1:12">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="22">
+      <c r="F8" s="20"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="21">
         <f>SUM(G8:G12)</f>
         <v>16</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="29">
         <v>16</v>
       </c>
-      <c r="J8" s="35"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="37"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="32"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="63" customHeight="1" spans="1:12">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="19" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="37"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="32"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="19" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="18">
         <v>12</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="37"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="32"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="19" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="37"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="32"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="75" customHeight="1" spans="1:12">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="19" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="19">
+      <c r="F12" s="20"/>
+      <c r="G12" s="18">
         <v>4</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="37"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="32"/>
     </row>
     <row r="13" s="1" customFormat="1" ht="72" customHeight="1" spans="1:12">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="18">
         <v>28</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="21">
         <f>SUM(G13:G17)</f>
         <v>72</v>
       </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="35">
+      <c r="I13" s="29"/>
+      <c r="J13" s="30">
         <v>72</v>
       </c>
-      <c r="K13" s="36"/>
-      <c r="L13" s="37"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="32"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="63" customHeight="1" spans="1:12">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="19" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="37"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="32"/>
     </row>
     <row r="15" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="19" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="37"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="32"/>
     </row>
     <row r="16" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="19" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="18">
         <v>28</v>
       </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="37"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="32"/>
     </row>
     <row r="17" s="1" customFormat="1" ht="75" customHeight="1" spans="1:12">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="19" t="s">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="19">
+      <c r="F17" s="20"/>
+      <c r="G17" s="18">
         <v>16</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="37"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="32"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="72" customHeight="1" spans="1:12">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="22">
+      <c r="F18" s="20"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="21">
         <f>SUM(G18:G22)</f>
         <v>16</v>
       </c>
-      <c r="I18" s="34"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="36">
+      <c r="I18" s="29"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="31">
         <v>16</v>
       </c>
-      <c r="L18" s="37"/>
+      <c r="L18" s="32"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="63" customHeight="1" spans="1:12">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="19" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="37"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="32"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="19" t="s">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="37"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="32"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="19" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="37"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="32"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="75" customHeight="1" spans="1:12">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="19" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="18">
         <v>16</v>
       </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="37"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="32"/>
     </row>
     <row r="23" s="2" customFormat="1"/>
     <row r="24" s="1" customFormat="1" ht="72" customHeight="1" spans="1:12">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="34" t="s">
+      <c r="F24" s="20"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="J24" s="35"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="37"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="32"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="63" customHeight="1" spans="1:12">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="19" t="s">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="37"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="32"/>
     </row>
     <row r="26" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="19" t="s">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="37"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="32"/>
     </row>
     <row r="27" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="19" t="s">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="37"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="32"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="75" customHeight="1" spans="1:12">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="19" t="s">
+      <c r="A28" s="15"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="37"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="32"/>
     </row>
     <row r="29" s="1" customFormat="1" ht="72" customHeight="1" spans="1:12">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="19">
+      <c r="F29" s="20"/>
+      <c r="G29" s="18">
         <v>12</v>
       </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="36">
+      <c r="H29" s="21"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="31">
         <v>48</v>
       </c>
-      <c r="L29" s="37"/>
+      <c r="L29" s="32"/>
     </row>
     <row r="30" s="1" customFormat="1" ht="63" customHeight="1" spans="1:12">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="19" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="37"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="32"/>
     </row>
     <row r="31" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="19" t="s">
+      <c r="A31" s="15"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="37"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="32"/>
     </row>
     <row r="32" s="1" customFormat="1" ht="67" customHeight="1" spans="1:12">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="19" t="s">
+      <c r="A32" s="15"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F32" s="21"/>
-      <c r="G32" s="19">
+      <c r="F32" s="20"/>
+      <c r="G32" s="18">
         <v>20</v>
       </c>
-      <c r="H32" s="22"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="37"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="32"/>
     </row>
     <row r="33" s="1" customFormat="1" ht="75" customHeight="1" spans="1:12">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="19" t="s">
+      <c r="A33" s="15"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="21" t="s">
+      <c r="E33" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="19">
+      <c r="F33" s="20"/>
+      <c r="G33" s="18">
         <v>16</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="37"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="32"/>
     </row>
     <row r="34" s="2" customFormat="1"/>
     <row r="35" ht="66" customHeight="1" spans="1:12">
@@ -2324,26 +2330,26 @@
       <c r="B35" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28">
+      <c r="F35" s="24"/>
+      <c r="G35" s="24">
         <v>3</v>
       </c>
-      <c r="H35" s="28"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="42">
+      <c r="H35" s="24"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37">
         <v>3</v>
       </c>
-      <c r="L35" s="26"/>
+      <c r="L35" s="22"/>
     </row>
     <row r="36" ht="71" customHeight="1" spans="1:11">
       <c r="A36" s="2" t="s">
@@ -2352,39 +2358,39 @@
       <c r="B36" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="F36" s="28" t="s">
+      <c r="F36" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43" t="s">
+      <c r="I36" s="38"/>
+      <c r="J36" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="K36" s="43"/>
+      <c r="K36" s="38"/>
     </row>
     <row r="37" ht="105" customHeight="1" spans="2:11">
       <c r="B37" s="5"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="29" t="s">
+      <c r="C37" s="22"/>
+      <c r="D37" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="28" t="s">
+      <c r="E37" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="28" t="s">
+      <c r="F37" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
     </row>
     <row r="38" ht="72" customHeight="1" spans="1:11">
       <c r="A38" s="2" t="s">
@@ -2393,19 +2399,19 @@
       <c r="B38" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F38" s="28"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="42">
+      <c r="F38" s="24"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37">
         <v>2</v>
       </c>
     </row>
@@ -2416,22 +2422,22 @@
       <c r="B39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="27" t="s">
+      <c r="D39" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="E39" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F39" s="28"/>
+      <c r="F39" s="24"/>
       <c r="G39" s="4">
         <v>16</v>
       </c>
-      <c r="I39" s="42"/>
-      <c r="J39" s="42"/>
-      <c r="K39" s="42">
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37">
         <v>16</v>
       </c>
     </row>
@@ -2445,9 +2451,9 @@
       <c r="D41" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-      <c r="K41" s="42">
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37">
         <v>32</v>
       </c>
     </row>
@@ -2464,20 +2470,20 @@
       <c r="D42" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="F42" s="28" t="s">
+      <c r="F42" s="24" t="s">
         <v>77</v>
       </c>
       <c r="G42" s="4">
         <v>18</v>
       </c>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42">
+      <c r="I42" s="37"/>
+      <c r="J42" s="37">
         <v>18</v>
       </c>
-      <c r="K42" s="42"/>
+      <c r="K42" s="37"/>
     </row>
     <row r="43" ht="69" spans="1:11">
       <c r="A43" s="2" t="s">
@@ -2489,9 +2495,9 @@
       <c r="C43" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="37"/>
     </row>
     <row r="45" spans="9:11">
       <c r="I45" s="5">
@@ -2507,8 +2513,118 @@
         <v>117</v>
       </c>
     </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6">
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+    </row>
+    <row r="50" spans="4:6">
+      <c r="D50" s="23"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+    </row>
+    <row r="51" spans="4:6">
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+    </row>
+    <row r="52" spans="4:6">
+      <c r="D52" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+    </row>
+    <row r="53" spans="4:6">
+      <c r="D53" s="23"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+    </row>
+    <row r="54" spans="4:6">
+      <c r="D54" s="23"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+    </row>
+    <row r="55" spans="4:6">
+      <c r="D55" s="23"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+    </row>
+    <row r="56" spans="4:6">
+      <c r="D56" s="23"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+    </row>
+    <row r="57" spans="4:6">
+      <c r="D57" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+    </row>
+    <row r="58" spans="4:6">
+      <c r="D58" s="23"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+    </row>
+    <row r="59" spans="4:6">
+      <c r="D59" s="23"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+    </row>
+    <row r="60" spans="4:6">
+      <c r="D60" s="23"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+    </row>
+    <row r="61" spans="4:6">
+      <c r="D61" s="23"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+    </row>
+    <row r="62" spans="4:6">
+      <c r="D62" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+    </row>
+    <row r="63" spans="4:6">
+      <c r="D63" s="23"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+    </row>
+    <row r="64" spans="4:6">
+      <c r="D64" s="23"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+    </row>
+    <row r="65" spans="4:6">
+      <c r="D65" s="23"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+    </row>
+    <row r="66" spans="4:6">
+      <c r="D66" s="23"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="65">
+  <mergeCells count="81">
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A23:XFD23"/>
     <mergeCell ref="A34:XFD34"/>
@@ -2536,8 +2652,24 @@
     <mergeCell ref="C24:C28"/>
     <mergeCell ref="C29:C33"/>
     <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="D52:D56"/>
+    <mergeCell ref="D57:D61"/>
+    <mergeCell ref="D62:D66"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="E52:E56"/>
+    <mergeCell ref="E57:E61"/>
+    <mergeCell ref="E62:E66"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="F48:F51"/>
+    <mergeCell ref="F52:F56"/>
+    <mergeCell ref="F57:F61"/>
+    <mergeCell ref="F62:F66"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="G57:G61"/>
+    <mergeCell ref="G62:G66"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="H3:H7"/>
     <mergeCell ref="H8:H12"/>

</xml_diff>